<commit_message>
update 16 Febuari 2018
</commit_message>
<xml_diff>
--- a/assets/excel/template_pelanggan.xlsx
+++ b/assets/excel/template_pelanggan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>id loket</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nama pelanggan</t>
   </si>
@@ -38,7 +35,22 @@
     <t>kode tarif</t>
   </si>
   <si>
-    <t>kwhterbaru</t>
+    <t>Gardu</t>
+  </si>
+  <si>
+    <t>provinsi</t>
+  </si>
+  <si>
+    <t>kabupaten</t>
+  </si>
+  <si>
+    <t>kecamatan</t>
+  </si>
+  <si>
+    <t>kelurahan</t>
+  </si>
+  <si>
+    <t>kodepos</t>
   </si>
 </sst>
 </file>
@@ -89,9 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,33 +419,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>